<commit_message>
Interfaz Demo (Sin json) y otras cositas varias.
</commit_message>
<xml_diff>
--- a/data/Iteracion2/ModeloRelacional.xlsx
+++ b/data/Iteracion2/ModeloRelacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\Pictures\Sistrans\Sistrans-D01\data\Iteracion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{18967C2E-E75F-4082-B681-219EEE26A63D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6DBE8C8-AE2F-42EA-8EA9-63B706F5F845}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="115">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -156,9 +156,6 @@
     <t>documentoPN</t>
   </si>
   <si>
-    <t>tipoDocPN</t>
-  </si>
-  <si>
     <t>PERSONANATURAL</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>PK, FK.ESTANTE.id, SA</t>
   </si>
   <si>
-    <t>FK_PERSONANATURAL.tipoDocumento, NC, UA</t>
-  </si>
-  <si>
     <t>NN, NC, DD, CK</t>
   </si>
   <si>
@@ -364,6 +358,18 @@
   </si>
   <si>
     <t>TIPO_PRODUCTO</t>
+  </si>
+  <si>
+    <t>NN, UA, CK</t>
+  </si>
+  <si>
+    <t>sucursal</t>
+  </si>
+  <si>
+    <t>FK_SUCURSAL.id, UA, NN, NC</t>
+  </si>
+  <si>
+    <t>NN, DD, CK</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="10" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1"/>
@@ -592,31 +598,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,6 +631,12 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,6 +648,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -956,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,33 +977,33 @@
     <col min="10" max="10" width="39" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1047,12 +1052,12 @@
         <v>17</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>25</v>
@@ -1091,39 +1096,39 @@
         <v>23</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
-      <c r="H6" s="23" t="s">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="H6" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
       <c r="M6" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="R6" s="27"/>
+      <c r="Q6" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="R6" s="18"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -1139,7 +1144,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>27</v>
@@ -1151,7 +1156,7 @@
         <v>29</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>3</v>
@@ -1160,15 +1165,15 @@
         <v>3</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>23</v>
@@ -1177,13 +1182,13 @@
         <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>23</v>
@@ -1192,43 +1197,39 @@
         <v>25</v>
       </c>
       <c r="K8" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
-      <c r="H10" s="35" t="s">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
+      <c r="H10" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
-      <c r="L10" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="M10" s="22"/>
-      <c r="O10" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="30"/>
+      <c r="L10" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -1244,7 +1245,7 @@
         <v>24</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>31</v>
@@ -1253,27 +1254,21 @@
         <v>28</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>109</v>
+        <v>56</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>23</v>
@@ -1282,45 +1277,44 @@
         <v>23</v>
       </c>
       <c r="E12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>98</v>
-      </c>
       <c r="H12" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="O12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="30"/>
+      <c r="L14" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="37"/>
+      <c r="M14" s="27"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
@@ -1339,15 +1333,24 @@
         <v>36</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>23</v>
@@ -1361,77 +1364,85 @@
       <c r="G16" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="L16" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="38"/>
-      <c r="E18" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="18"/>
-      <c r="H18" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="23"/>
+      <c r="B18" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="E18" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="33"/>
+      <c r="H18" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="26"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>46</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="I22" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="21"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="I22" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="36"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
@@ -1449,11 +1460,8 @@
       <c r="F23" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="15" t="s">
-        <v>43</v>
-      </c>
       <c r="I23" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J23" s="10" t="s">
         <v>28</v>
@@ -1462,15 +1470,15 @@
         <v>14</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>25</v>
@@ -1479,16 +1487,13 @@
         <v>23</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J24" s="10" t="s">
         <v>23</v>
@@ -1500,134 +1505,134 @@
         <v>32</v>
       </c>
       <c r="M24" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="I26" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
+      <c r="B26" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="I26" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="J26" s="25"/>
+      <c r="K26" s="25"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="25"/>
+      <c r="N26" s="25"/>
+      <c r="O26" s="25"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K27" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="K27" s="10" t="s">
+      <c r="L27" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="L27" s="10" t="s">
+      <c r="M27" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="N27" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="M27" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="N27" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="O27" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="I28" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K28" s="10" t="s">
         <v>25</v>
       </c>
       <c r="L28" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O28" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
+      <c r="B30" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="H31" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="I31" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>25</v>
@@ -1639,68 +1644,73 @@
         <v>25</v>
       </c>
       <c r="F32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H32" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>59</v>
-      </c>
       <c r="I32" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="F34" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="G34" s="31"/>
+      <c r="B34" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="F34" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="22"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>59</v>
+      <c r="D36" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G36" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="I22:M22"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="L10:N10"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="B34:D34"/>
@@ -1708,18 +1718,13 @@
     <mergeCell ref="B30:J30"/>
     <mergeCell ref="I26:O26"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L14:N14"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B22:G22"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I22:M22"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="H18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ya funciona agregar producto :D
</commit_message>
<xml_diff>
--- a/data/Iteracion2/ModeloRelacional.xlsx
+++ b/data/Iteracion2/ModeloRelacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\Pictures\Sistrans\Sistrans-D01\data\Iteracion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D6DBE8C8-AE2F-42EA-8EA9-63B706F5F845}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FD302806-0F13-4832-84A0-37E65D31611B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>NN, DD, CK</t>
+  </si>
+  <si>
+    <t>CK, NN, UA</t>
   </si>
 </sst>
 </file>
@@ -598,6 +601,24 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -631,12 +652,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,18 +669,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -961,8 +964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,24 +989,24 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1078,16 +1081,16 @@
         <v>23</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>23</v>
@@ -1106,29 +1109,29 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="30"/>
-      <c r="H6" s="26" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
+      <c r="H6" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
       <c r="M6" s="13" t="s">
         <v>2</v>
       </c>
       <c r="O6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="R6" s="18"/>
+      <c r="R6" s="24"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
@@ -1213,23 +1216,23 @@
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
-      <c r="H10" s="28" t="s">
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34"/>
+      <c r="H10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="30"/>
-      <c r="L10" s="27" t="s">
+      <c r="I10" s="33"/>
+      <c r="J10" s="34"/>
+      <c r="L10" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
@@ -1302,19 +1305,19 @@
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
-      <c r="L14" s="27" t="s">
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="L14" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
@@ -1375,18 +1378,18 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="E18" s="32" t="s">
+      <c r="C18" s="35"/>
+      <c r="E18" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="H18" s="26" t="s">
+      <c r="F18" s="37"/>
+      <c r="H18" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="26"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
@@ -1429,20 +1432,20 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="I22" s="34" t="s">
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="I22" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="36"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="17"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
@@ -1498,8 +1501,8 @@
       <c r="J24" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="10" t="s">
-        <v>23</v>
+      <c r="K24" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>32</v>
@@ -1509,20 +1512,20 @@
       </c>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
-      <c r="I26" s="24" t="s">
+      <c r="C26" s="22"/>
+      <c r="D26" s="23"/>
+      <c r="I26" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="31"/>
+      <c r="O26" s="31"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
@@ -1589,17 +1592,17 @@
       </c>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
@@ -1660,15 +1663,15 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="F34" s="21" t="s">
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="F34" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="22"/>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
@@ -1706,11 +1709,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="I22:M22"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="L10:N10"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="B34:D34"/>
@@ -1725,6 +1723,11 @@
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="E18:F18"/>
+    <mergeCell ref="I22:M22"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="L10:N10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Aún no termino el documento
</commit_message>
<xml_diff>
--- a/data/Iteracion2/ModeloRelacional.xlsx
+++ b/data/Iteracion2/ModeloRelacional.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estudiante\Pictures\Sistrans\Sistrans-D01\data\Iteracion2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Universidad\4toSemestre\Sistrans\Iteraciones\Iteración2\Proyecto eclipse\Sistrans-D01\data\Iteracion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FD302806-0F13-4832-84A0-37E65D31611B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="154">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -373,12 +372,126 @@
   </si>
   <si>
     <t>CK, NN, UA</t>
+  </si>
+  <si>
+    <t>VARCHAR2(100BYTE)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(50BYTE)</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>VARCHAR2(250BYTE)</t>
+  </si>
+  <si>
+    <t>NUMBER(*,8)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(10BYTE)</t>
+  </si>
+  <si>
+    <t>NUMBER(*,1)</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>VARCHAR2(100 BYTE)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(255 BYTE)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(200 BYTE)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(150 BYTE)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(13 BYTE)</t>
+  </si>
+  <si>
+    <t>NUMBER(*)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(13BYTE)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(255BYTE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR2(200 BYTE) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMBER(*) </t>
+  </si>
+  <si>
+    <t>NUMBER(1)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUMBER(*,1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VARCHAR2(255 BYTE) </t>
+  </si>
+  <si>
+    <t>promDescSegunda</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>unidadesDisponibles</t>
+  </si>
+  <si>
+    <t>unidadesVendidas</t>
+  </si>
+  <si>
+    <t>fechaInicio</t>
+  </si>
+  <si>
+    <t>fechaFin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">descuento </t>
+  </si>
+  <si>
+    <t>PK,NN</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>FK (producto.codigoBarras) , NN</t>
+  </si>
+  <si>
+    <t>promPagLleveCanti</t>
+  </si>
+  <si>
+    <t>pague</t>
+  </si>
+  <si>
+    <t>lleve</t>
+  </si>
+  <si>
+    <t>NN,UA</t>
+  </si>
+  <si>
+    <t>promDescuento</t>
+  </si>
+  <si>
+    <t>promPagLleveUnidad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -536,39 +649,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -585,7 +665,7 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="10" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1"/>
@@ -597,70 +677,29 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="12" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="11" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -669,6 +708,66 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -961,23 +1060,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:R36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.5703125" bestFit="1" customWidth="1"/>
@@ -986,748 +1085,1395 @@
     <col min="17" max="17" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O5" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="Q5" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-      <c r="H6" s="19" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="H8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="M6" s="13" t="s">
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="M8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="O8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="24" t="s">
+      <c r="Q8" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="R6" s="24"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="R8" s="17"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="23"/>
+      <c r="M9" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="N9" s="23"/>
+      <c r="O9" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="R9" s="24" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="Q10" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="R10" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E11" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R11" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B10" s="32" t="s">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
-      <c r="H10" s="32" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="H13" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
-      <c r="L10" s="18" t="s">
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="L13" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
+      <c r="B14" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="I14" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K14" s="23"/>
+      <c r="L14" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M15" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J16" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M16" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B14" s="32" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="34"/>
-      <c r="L14" s="18" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="I19" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="L20" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="23"/>
+      <c r="B21" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C21" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D21" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E21" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F21" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G21" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="H21" s="23"/>
+      <c r="I21" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="M21" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="N21" s="24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="M22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B25" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="E25" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="13"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="23"/>
+      <c r="B26" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="F28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="6" t="s">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B31" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="27"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B32" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="F32" s="33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E34" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="I38" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H42" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I42" s="15"/>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H43" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="I43" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="J43" s="34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H44" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H45" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="F48" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="23"/>
+      <c r="F49" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="G49" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="D51" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="E55" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="F55" s="35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="D57" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E57" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="M16" s="3" t="s">
+      <c r="F57" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="F61" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="G61" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+      <c r="I66" s="20"/>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F68" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G68" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="H68" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="I68" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C69" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="E18" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="37"/>
-      <c r="H18" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="I22" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="17"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L23" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="M23" s="10" t="s">
+      <c r="D69" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E69" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="F69" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H69" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="I69" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="J69" s="37"/>
+      <c r="K69" s="37"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="39"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="39"/>
+      <c r="J71" s="39"/>
+      <c r="K71" s="39"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="E73" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F73" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G73" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="H73" s="38" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="I73" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="J73" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="K73" s="38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C74" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E74" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="F74" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="L24" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M24" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
-      <c r="I26" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="9" t="s">
+      <c r="G74" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H74" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="I74" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="J74" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="K74" s="38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C76" s="41"/>
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
+      <c r="F76" s="41"/>
+      <c r="G76" s="41"/>
+      <c r="H76" s="41"/>
+      <c r="I76" s="42"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J77" s="37"/>
+      <c r="K77" s="37"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D78" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F78" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G78" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="H78" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I78" s="38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D79" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E79" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="F79" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="H79" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="I79" s="38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C81" s="41"/>
+      <c r="D81" s="41"/>
+      <c r="E81" s="41"/>
+      <c r="F81" s="41"/>
+      <c r="G81" s="41"/>
+      <c r="H81" s="41"/>
+      <c r="I81" s="41"/>
+      <c r="J81" s="41"/>
+      <c r="K81" s="42"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="37"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="37"/>
+      <c r="K82" s="37"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="K27" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L27" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="M27" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="N27" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="O27" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I28" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="K28" s="10" t="s">
+      <c r="C83" s="38" t="s">
+        <v>139</v>
+      </c>
+      <c r="D83" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="E83" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F83" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="G83" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="H83" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="I83" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="J83" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="K83" s="38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="C84" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D84" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="E84" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="F84" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="L28" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="M28" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="N28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="O28" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="G84" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="H84" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="I84" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="J84" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="F34" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="G34" s="28"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>85</v>
-      </c>
+      <c r="K84" s="38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J85" s="37"/>
+      <c r="K85" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="I26:O26"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="L14:N14"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="I22:M22"/>
+  <mergeCells count="22">
+    <mergeCell ref="B81:K81"/>
+    <mergeCell ref="B66:I66"/>
+    <mergeCell ref="B71:K71"/>
+    <mergeCell ref="B76:I76"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H13:J13"/>
     <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="L10:N10"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="L13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Documento, tablas de Excel actualizadas y con tipos.
</commit_message>
<xml_diff>
--- a/data/Iteracion2/ModeloRelacional.xlsx
+++ b/data/Iteracion2/ModeloRelacional.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="155">
   <si>
     <t>PRODUCTO</t>
   </si>
@@ -440,9 +440,6 @@
     <t xml:space="preserve">VARCHAR2(255 BYTE) </t>
   </si>
   <si>
-    <t>promDescSegunda</t>
-  </si>
-  <si>
     <t>descripcion</t>
   </si>
   <si>
@@ -470,9 +467,6 @@
     <t>FK (producto.codigoBarras) , NN</t>
   </si>
   <si>
-    <t>promPagLleveCanti</t>
-  </si>
-  <si>
     <t>pague</t>
   </si>
   <si>
@@ -482,10 +476,19 @@
     <t>NN,UA</t>
   </si>
   <si>
-    <t>promDescuento</t>
-  </si>
-  <si>
-    <t>promPagLleveUnidad</t>
+    <t>PROM_PAGLLEVECANT</t>
+  </si>
+  <si>
+    <t>PROM_PAGLLEVEUNID</t>
+  </si>
+  <si>
+    <t>PROM_SEGUNIDESCUENTO</t>
+  </si>
+  <si>
+    <t>PROM_DESCUENTO</t>
+  </si>
+  <si>
+    <t>VARCHAR2(250 BYTE)</t>
   </si>
 </sst>
 </file>
@@ -682,6 +685,75 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -691,83 +763,14 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="8" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="12" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1061,29 +1064,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R85"/>
+  <dimension ref="A2:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="23" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -1095,78 +1100,78 @@
     <col min="28" max="28" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="F3" s="24" t="s">
+      <c r="E3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="H3" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" s="24" t="s">
+      <c r="H3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="N3" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="O3" s="24" t="s">
+      <c r="N3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="Q3" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q3" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1216,7 +1221,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>80</v>
       </c>
@@ -1266,78 +1271,68 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B8" s="18" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="H8" s="18" t="s">
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="H8" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
       <c r="M8" s="12" t="s">
         <v>2</v>
       </c>
       <c r="O8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="Q8" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="R8" s="17"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
       <c r="B9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="E9" s="29" t="s">
+      <c r="C9" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>124</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="29" t="s">
+      <c r="G9" s="14"/>
+      <c r="H9" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="J9" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="K9" s="29" t="s">
+      <c r="K9" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="24" t="s">
+      <c r="L9" s="14"/>
+      <c r="M9" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="N9" s="23"/>
-      <c r="O9" s="24" t="s">
+      <c r="N9" s="14"/>
+      <c r="O9" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="R9" s="24" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P9" s="14"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>20</v>
       </c>
@@ -1371,14 +1366,8 @@
       <c r="O10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>79</v>
       </c>
@@ -1412,71 +1401,75 @@
       <c r="O11" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Q11" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="R11" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B13" s="18" t="s">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="H13" s="18" t="s">
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="H13" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="L13" s="19" t="s">
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="L13" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="29" t="s">
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="P13" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q13" s="42"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="F14" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="I14" s="29" t="s">
+      <c r="F14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="I14" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="J14" s="29" t="s">
+      <c r="J14" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="M14" s="24" t="s">
+      <c r="K14" s="14"/>
+      <c r="L14" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="M14" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="N14" s="24" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N14" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q14" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>20</v>
       </c>
@@ -1510,8 +1503,14 @@
       <c r="N15" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>79</v>
       </c>
@@ -1545,20 +1544,26 @@
       <c r="N16" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="P16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="I19" s="18" t="s">
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="I19" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="J19" s="18"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -1585,47 +1590,47 @@
       <c r="J20" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="L20" s="19" t="s">
+      <c r="L20" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="29" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="29" t="s">
+      <c r="G21" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="23"/>
-      <c r="I21" s="29" t="s">
+      <c r="H21" s="14"/>
+      <c r="I21" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="K21" s="23"/>
-      <c r="L21" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="M21" s="24" t="s">
-        <v>118</v>
-      </c>
-      <c r="N21" s="24" t="s">
+      <c r="K21" s="14"/>
+      <c r="L21" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="M21" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="N21" s="15" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1676,36 +1681,46 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="36"/>
       <c r="E25" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F25" s="13"/>
+      <c r="H25" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="33" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="33" t="s">
+      <c r="D26" s="14"/>
+      <c r="E26" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="K26" s="14"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
@@ -1720,6 +1735,15 @@
       <c r="F27" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
@@ -1734,31 +1758,58 @@
       <c r="F28" s="8" t="s">
         <v>48</v>
       </c>
+      <c r="H28" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H30" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="I30" s="30"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="27"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="34"/>
+      <c r="H31" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="I31" s="16" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="33" t="s">
+      <c r="D32" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="F32" s="18" t="s">
         <v>124</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -1777,6 +1828,12 @@
       <c r="F33" s="7" t="s">
         <v>42</v>
       </c>
+      <c r="H33" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
@@ -1796,44 +1853,44 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="15"/>
-      <c r="J37" s="16"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="C38" s="34" t="s">
+      <c r="B38" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E38" s="34" t="s">
+      <c r="E38" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F38" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" s="34" t="s">
+      <c r="F38" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G38" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="I38" s="34" t="s">
+      <c r="I38" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="J38" s="34" t="s">
+      <c r="J38" s="19" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1896,24 +1953,61 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H42" s="14" t="s">
+      <c r="B42" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="41"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+      <c r="H42" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="16"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H43" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" s="34" t="s">
+      <c r="B43" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D43" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="I43" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="J43" s="34" t="s">
+      <c r="J43" s="19" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="H44" s="4" t="s">
         <v>60</v>
       </c>
@@ -1925,6 +2019,21 @@
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>85</v>
+      </c>
       <c r="H45" s="9" t="s">
         <v>84</v>
       </c>
@@ -1935,545 +2044,520 @@
         <v>85</v>
       </c>
     </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B47" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="41"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+    </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="30"/>
-      <c r="D48" s="30"/>
-      <c r="F48" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="G48" s="31"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="28" t="s">
+      <c r="B48" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="G48" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="C49" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="28" t="s">
-        <v>124</v>
-      </c>
-      <c r="G49" s="28" t="s">
+      <c r="H48" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="26"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H53" s="18" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G50" s="2" t="s">
+      <c r="I53" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="J53" s="22"/>
+      <c r="K53" s="22"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F54" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H54" s="23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D51" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="G51" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="32"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="E55" s="36" t="s">
+      <c r="I54" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H55" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="27" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F58" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="F55" s="35" t="s">
+      <c r="G58" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H58" s="18" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" s="10" t="s">
+      <c r="I58" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E59" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F59" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H59" s="23" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C57" s="10" t="s">
+      <c r="I59" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D57" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="C60" s="32"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="C61" s="35" t="s">
+      <c r="D60" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E60" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F60" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I60" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="28"/>
+      <c r="F62" s="28"/>
+      <c r="G62" s="28"/>
+      <c r="H62" s="28"/>
+      <c r="I62" s="28"/>
+      <c r="J62" s="28"/>
+      <c r="K62" s="28"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F63" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="35" t="s">
+      <c r="G63" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="E61" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="F61" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="G61" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="H61" s="35" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="10" t="s">
+      <c r="H63" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I63" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="J63" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K63" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C62" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="H62" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D63" s="10" t="s">
+      <c r="C64" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="E64" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="F64" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G64" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H64" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I64" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="J64" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="K64" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E65" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F65" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F63" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="G63" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H63" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" s="20" t="s">
+      <c r="G65" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H65" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I65" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J65" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K65" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28"/>
+      <c r="G67" s="28"/>
+      <c r="H67" s="28"/>
+      <c r="I67" s="28"/>
+      <c r="J67" s="28"/>
+      <c r="K67" s="28"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="F68" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G68" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H68" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="I68" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="J68" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K68" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C69" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="20"/>
-      <c r="H66" s="20"/>
-      <c r="I66" s="20"/>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J67" s="37"/>
-      <c r="K67" s="37"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C68" s="38" t="s">
+      <c r="D69" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="D68" s="38" t="s">
+      <c r="E69" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E68" s="38" t="s">
+      <c r="F69" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="F68" s="38" t="s">
+      <c r="G69" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="G68" s="38" t="s">
+      <c r="H69" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="I69" s="23" t="s">
         <v>143</v>
       </c>
-      <c r="H68" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="I68" s="38" t="s">
+      <c r="J69" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="K69" s="23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="J68" s="37"/>
-      <c r="K68" s="37"/>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B69" s="38" t="s">
+      <c r="C70" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D70" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="C69" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D69" s="38" t="s">
+      <c r="E70" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F70" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H70" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="E69" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="F69" s="38" t="s">
+      <c r="I70" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G69" s="38" t="s">
+      <c r="J70" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H69" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="I69" s="38" t="s">
+      <c r="K70" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J69" s="37"/>
-      <c r="K69" s="37"/>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B71" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="C71" s="39"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="39"/>
-      <c r="K71" s="39"/>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B73" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C73" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="D73" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="E73" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="F73" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="G73" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="H73" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="I73" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="J73" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="K73" s="38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="C74" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="E74" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="F74" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G74" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H74" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="I74" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="J74" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="K74" s="38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B76" s="40" t="s">
-        <v>152</v>
-      </c>
-      <c r="C76" s="41"/>
-      <c r="D76" s="41"/>
-      <c r="E76" s="41"/>
-      <c r="F76" s="41"/>
-      <c r="G76" s="41"/>
-      <c r="H76" s="41"/>
-      <c r="I76" s="42"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J77" s="37"/>
-      <c r="K77" s="37"/>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B78" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C78" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="D78" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="E78" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="F78" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="G78" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="H78" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="I78" s="38" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B79" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="C79" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D79" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="E79" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="F79" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H79" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="I79" s="38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="C81" s="41"/>
-      <c r="D81" s="41"/>
-      <c r="E81" s="41"/>
-      <c r="F81" s="41"/>
-      <c r="G81" s="41"/>
-      <c r="H81" s="41"/>
-      <c r="I81" s="41"/>
-      <c r="J81" s="41"/>
-      <c r="K81" s="42"/>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82" s="37"/>
-      <c r="C82" s="37"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="37"/>
-      <c r="G82" s="37"/>
-      <c r="H82" s="37"/>
-      <c r="I82" s="37"/>
-      <c r="J82" s="37"/>
-      <c r="K82" s="37"/>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="C83" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="D83" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="E83" s="38" t="s">
-        <v>141</v>
-      </c>
-      <c r="F83" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="G83" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="H83" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="I83" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="J83" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="K83" s="38" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="C84" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D84" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="E84" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="F84" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G84" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="H84" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="I84" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="J84" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="K84" s="38" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J85" s="37"/>
-      <c r="K85" s="37"/>
+    </row>
+    <row r="85" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="J85" s="22"/>
+      <c r="K85" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B81:K81"/>
-    <mergeCell ref="B66:I66"/>
-    <mergeCell ref="B71:K71"/>
-    <mergeCell ref="B76:I76"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H42:J42"/>
     <mergeCell ref="L20:N20"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B37:J37"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="L13:N13"/>
+    <mergeCell ref="B62:K62"/>
+    <mergeCell ref="B57:I57"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="B67:K67"/>
+    <mergeCell ref="B52:I52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cosas para poblar las tablas
</commit_message>
<xml_diff>
--- a/data/Iteracion2/ModeloRelacional.xlsx
+++ b/data/Iteracion2/ModeloRelacional.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Universidad\4toSemestre\Sistrans\Iteraciones\Iteración2\Proyecto eclipse\Sistrans-D01\data\Iteracion2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Universidad\4toSemestre\Sistrans\Iteraciones\Iteración3\Sistrans-D01\data\Iteracion2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -350,9 +350,6 @@
     <t>codigoBarrasProducto</t>
   </si>
   <si>
-    <t>estaEnPromocion</t>
-  </si>
-  <si>
     <t>UA, NN, CK</t>
   </si>
   <si>
@@ -489,6 +486,9 @@
   </si>
   <si>
     <t>VARCHAR2(250 BYTE)</t>
+  </si>
+  <si>
+    <t>estaPromocion</t>
   </si>
 </sst>
 </file>
@@ -715,6 +715,54 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,54 +771,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="7" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,74 +1101,74 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="14"/>
       <c r="B3" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="G3" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="H3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" s="15" t="s">
+      <c r="K3" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="L3" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="M3" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="M3" s="15" t="s">
+      <c r="N3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="O3" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="N3" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>123</v>
-      </c>
       <c r="P3" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1202,10 +1202,10 @@
       <c r="K4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -1217,8 +1217,8 @@
       <c r="P4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>108</v>
+      <c r="Q4" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1268,23 +1268,23 @@
         <v>70</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="H8" s="40" t="s">
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="H8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
-      <c r="K8" s="40"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
       <c r="M8" s="12" t="s">
         <v>2</v>
       </c>
@@ -1295,40 +1295,40 @@
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I9" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>129</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>130</v>
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N9" s="14"/>
       <c r="O9" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P9" s="14"/>
     </row>
@@ -1403,70 +1403,70 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="H13" s="40" t="s">
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="H13" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="L13" s="31" t="s">
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="L13" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="P13" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q13" s="42"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="P13" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q13" s="26"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I14" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="J14" s="17" t="s">
         <v>129</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>130</v>
       </c>
       <c r="K14" s="14"/>
       <c r="L14" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M14" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N14" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P14" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q14" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1501,7 +1501,7 @@
         <v>56</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>107</v>
@@ -1542,7 +1542,7 @@
         <v>101</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>85</v>
@@ -1552,49 +1552,49 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="I19" s="40" t="s">
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="I19" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="J19" s="40"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="F20" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="L20" s="31" t="s">
+      <c r="L20" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
+      <c r="M20" s="25"/>
+      <c r="N20" s="25"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
@@ -1625,13 +1625,13 @@
       </c>
       <c r="K21" s="14"/>
       <c r="L21" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M21" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1681,44 +1681,44 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="36"/>
+      <c r="C25" s="35"/>
       <c r="E25" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F25" s="13"/>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I26" s="16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K26" s="14"/>
     </row>
@@ -1750,7 +1750,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>81</v>
@@ -1765,45 +1765,45 @@
         <v>37</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H30" s="30" t="s">
+      <c r="H30" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="I30" s="30"/>
+      <c r="I30" s="39"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
       <c r="H31" s="16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C32" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="D32" s="18" t="s">
-        <v>133</v>
-      </c>
       <c r="E32" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>65</v>
@@ -1853,45 +1853,45 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="38"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
-      <c r="J37" s="39"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="30"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E38" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="H38" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="F38" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>133</v>
-      </c>
       <c r="I38" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
@@ -1953,43 +1953,43 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="H42" s="37" t="s">
+      <c r="C42" s="27"/>
+      <c r="D42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="27"/>
+      <c r="H42" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I42" s="38"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F43" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="I43" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="H43" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" s="19" t="s">
+      <c r="J43" s="19" t="s">
         <v>129</v>
-      </c>
-      <c r="J43" s="19" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
@@ -2026,7 +2026,7 @@
         <v>23</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E45" s="10" t="s">
         <v>32</v>
@@ -2045,37 +2045,37 @@
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="27"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C48" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F48" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="G48" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="F48" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="G48" s="20" t="s">
-        <v>124</v>
-      </c>
       <c r="H48" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -2125,41 +2125,41 @@
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="26"/>
+      <c r="B52" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="41"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+      <c r="G52" s="41"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="42"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G53" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I53" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J53" s="22"/>
       <c r="K53" s="22"/>
@@ -2169,41 +2169,41 @@
         <v>20</v>
       </c>
       <c r="C54" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D54" s="23" t="s">
+      <c r="E54" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E54" s="23" t="s">
+      <c r="F54" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F54" s="23" t="s">
+      <c r="G54" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="G54" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="H54" s="23" t="s">
         <v>69</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J54" s="22"/>
       <c r="K54" s="22"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="C55" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D55" s="23" t="s">
-        <v>145</v>
-      </c>
       <c r="E55" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F55" s="23" t="s">
         <v>25</v>
@@ -2212,7 +2212,7 @@
         <v>25</v>
       </c>
       <c r="H55" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I55" s="23" t="s">
         <v>25</v>
@@ -2221,41 +2221,41 @@
       <c r="K55" s="22"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
+      <c r="B57" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G58" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H58" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I58" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
@@ -2263,39 +2263,39 @@
         <v>20</v>
       </c>
       <c r="C59" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D59" s="23" t="s">
+      <c r="E59" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E59" s="23" t="s">
+      <c r="F59" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F59" s="23" t="s">
+      <c r="G59" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="G59" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="H59" s="23" t="s">
         <v>69</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" s="23" t="s">
         <v>23</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F60" s="23" t="s">
         <v>25</v>
@@ -2304,56 +2304,56 @@
         <v>25</v>
       </c>
       <c r="H60" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I60" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="28"/>
-      <c r="F62" s="28"/>
-      <c r="G62" s="28"/>
-      <c r="H62" s="28"/>
-      <c r="I62" s="28"/>
-      <c r="J62" s="28"/>
-      <c r="K62" s="28"/>
+      <c r="B62" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="36"/>
+      <c r="J62" s="36"/>
+      <c r="K62" s="36"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H63" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I63" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K63" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
@@ -2361,45 +2361,45 @@
         <v>20</v>
       </c>
       <c r="C64" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D64" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D64" s="23" t="s">
+      <c r="E64" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E64" s="23" t="s">
+      <c r="F64" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F64" s="23" t="s">
+      <c r="G64" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="G64" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="H64" s="23" t="s">
         <v>69</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J64" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="K64" s="23" t="s">
         <v>147</v>
-      </c>
-      <c r="K64" s="23" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C65" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D65" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="C65" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D65" s="23" t="s">
-        <v>145</v>
-      </c>
       <c r="E65" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F65" s="23" t="s">
         <v>25</v>
@@ -2408,7 +2408,7 @@
         <v>25</v>
       </c>
       <c r="H65" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I65" s="23" t="s">
         <v>25</v>
@@ -2421,49 +2421,49 @@
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="28"/>
-      <c r="J67" s="28"/>
-      <c r="K67" s="28"/>
+      <c r="B67" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="36"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="36"/>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C68" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F68" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G68" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I68" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J68" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K68" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
@@ -2471,45 +2471,45 @@
         <v>20</v>
       </c>
       <c r="C69" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="D69" s="23" t="s">
+      <c r="E69" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="E69" s="23" t="s">
+      <c r="F69" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="F69" s="23" t="s">
+      <c r="G69" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="G69" s="23" t="s">
-        <v>142</v>
       </c>
       <c r="H69" s="23" t="s">
         <v>69</v>
       </c>
       <c r="I69" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J69" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="K69" s="23" t="s">
         <v>147</v>
-      </c>
-      <c r="K69" s="23" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="D70" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="C70" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="D70" s="23" t="s">
-        <v>145</v>
-      </c>
       <c r="E70" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F70" s="23" t="s">
         <v>25</v>
@@ -2518,7 +2518,7 @@
         <v>25</v>
       </c>
       <c r="H70" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I70" s="23" t="s">
         <v>25</v>
@@ -2536,18 +2536,8 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="L13:N13"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B67:K67"/>
+    <mergeCell ref="B52:I52"/>
     <mergeCell ref="L20:N20"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B25:C25"/>
@@ -2556,8 +2546,18 @@
     <mergeCell ref="B57:I57"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="H30:I30"/>
-    <mergeCell ref="B67:K67"/>
-    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="L13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>